<commit_message>
Empty fills and borders considered equal no matter what colors they are.
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Styles/StyleWorksheet.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Styles/StyleWorksheet.xlsx
@@ -49,7 +49,7 @@
       <x:family val="2"/>
     </x:font>
   </x:fonts>
-  <x:fills count="4">
+  <x:fills count="3">
     <x:fill>
       <x:patternFill patternType="none"/>
     </x:fill>
@@ -60,9 +60,6 @@
       <x:patternFill patternType="solid">
         <x:fgColor rgb="FF00FFFF"/>
       </x:patternFill>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="none"/>
     </x:fill>
   </x:fills>
   <x:borders count="1">
@@ -84,27 +81,20 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="3">
+  <x:cellStyleXfs count="2">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="3">
+  <x:cellXfs count="2">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -423,24 +413,24 @@
       </x:c>
     </x:row>
     <x:row r="2" spans="1:6">
-      <x:c r="A2" s="2" t="s">
+      <x:c r="A2" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:6" s="0" customFormat="1" ht="20" customHeight="1">
-      <x:c r="D4" s="2" t="s"/>
-      <x:c r="E4" s="2" t="s"/>
-      <x:c r="F4" s="2" t="s"/>
+      <x:c r="D4" s="0" t="s"/>
+      <x:c r="E4" s="0" t="s"/>
+      <x:c r="F4" s="0" t="s"/>
     </x:row>
     <x:row r="5" spans="1:6" s="0" customFormat="1" ht="20" customHeight="1">
-      <x:c r="D5" s="2" t="s"/>
-      <x:c r="E5" s="2" t="s"/>
-      <x:c r="F5" s="2" t="s"/>
+      <x:c r="D5" s="0" t="s"/>
+      <x:c r="E5" s="0" t="s"/>
+      <x:c r="F5" s="0" t="s"/>
     </x:row>
     <x:row r="6" spans="1:6" s="0" customFormat="1" ht="20" customHeight="1">
-      <x:c r="D6" s="2" t="s"/>
-      <x:c r="E6" s="2" t="s"/>
-      <x:c r="F6" s="2" t="s"/>
+      <x:c r="D6" s="0" t="s"/>
+      <x:c r="E6" s="0" t="s"/>
+      <x:c r="F6" s="0" t="s"/>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>